<commit_message>
NC92Soil Versione 0.7 bis del 23/09/2020
- Implementato variatore di curve di decadimento secondo il modello di Darendeli
- Implementata possibilità di specificare la variabilità delle curve di decadimento anche in fase di analisi batch con profili
</commit_message>
<xml_diff>
--- a/Batch analysis test.xlsx
+++ b/Batch analysis test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giaac\Documents\Repo Git\GitLab\SRA Software\GUI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B559AB15-E700-4805-A924-136BA32029C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4647BB3A-6A9C-4F6F-909C-4312DB20B123}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8964" xr2:uid="{4D2D38F4-E5D1-49A1-97A0-EF49BC19DD52}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4D2D38F4-E5D1-49A1-97A0-EF49BC19DD52}"/>
   </bookViews>
   <sheets>
     <sheet name="Stochastic" sheetId="7" r:id="rId1"/>
@@ -115,7 +115,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="49">
   <si>
     <t>Soil name</t>
   </si>
@@ -271,7 +271,7 @@
     <t>1.35^x + 250</t>
   </si>
   <si>
-    <t>2*x + 3*y</t>
+    <t>Darendeli</t>
   </si>
 </sst>
 </file>
@@ -662,7 +662,7 @@
   <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -742,8 +742,8 @@
       <c r="G2" t="s">
         <v>13</v>
       </c>
-      <c r="H2">
-        <v>1</v>
+      <c r="H2" t="s">
+        <v>48</v>
       </c>
       <c r="I2" s="5" t="s">
         <v>41</v>
@@ -777,11 +777,11 @@
       <c r="G3" t="s">
         <v>13</v>
       </c>
-      <c r="H3">
-        <v>1</v>
+      <c r="H3" t="s">
+        <v>48</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
@@ -806,8 +806,8 @@
       <c r="G4" t="s">
         <v>13</v>
       </c>
-      <c r="H4">
-        <v>1</v>
+      <c r="H4" t="s">
+        <v>48</v>
       </c>
       <c r="I4" s="5" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
NC92Soil versione 0.8 del 29/09/2020
- Implementata generazione automatica dei file di input batch dal file di input stocastico
- Implementata possibilità di lavorare più file di input batch contemporaneamente con creazione automatica dell'albero delle sottocartelle
- Implementata possiblità di plottare dinamicamente i profili analizzati
- Correzione di bug minori
</commit_message>
<xml_diff>
--- a/Batch analysis test.xlsx
+++ b/Batch analysis test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giaac\Documents\Repo Git\GitLab\SRA Software\GUI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4647BB3A-6A9C-4F6F-909C-4312DB20B123}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A0F72EF-F9E7-47DF-967C-E917AB1B841C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4D2D38F4-E5D1-49A1-97A0-EF49BC19DD52}"/>
   </bookViews>
@@ -661,8 +661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4957287E-A37F-4CE2-B169-A739F2ED3546}">
   <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -749,7 +749,7 @@
         <v>41</v>
       </c>
       <c r="M2">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="O2" t="s">
         <v>44</v>

</xml_diff>